<commit_message>
feat: Update of the variantconvert distribution (1.2.2 installed)
</commit_message>
<xml_diff>
--- a/Scoring_Criteria_AnnotSV_v3.3.xlsx
+++ b/Scoring_Criteria_AnnotSV_v3.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veron\Desktop\Tutu\AnnotSV ranking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958CBEF3-85D4-481C-8945-902890345149}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D27B94-FE22-4106-9EAF-80F3D1A49DD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="3615" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8190" windowHeight="3615" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loss" sheetId="1" r:id="rId1"/>
@@ -1864,13 +1864,13 @@
     <t>Table 2: AnnotSV (v3.2) implementation of the Gain CNV interpretation scoring metric</t>
   </si>
   <si>
-    <t>Table 1: AnnotSV (v3.2) implementation of the Loss CNV interpretation scoring metric</t>
-  </si>
-  <si>
     <t>In each section, only 1 “non-zero value” criterion (from the most pathogenic to the least) is assigned. “Zero value” criteria are all evaluated</t>
   </si>
   <si>
     <t>gnomAD_pLI, HI_DDDpercent</t>
+  </si>
+  <si>
+    <t>Table 1: AnnotSV (v3.3) implementation of the Loss CNV interpretation scoring metric</t>
   </si>
 </sst>
 </file>
@@ -2627,6 +2627,33 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2669,32 +2696,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2712,54 +2760,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2999,8 +2999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3013,29 +3013,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="80" t="s">
-        <v>180</v>
-      </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="82"/>
+      <c r="A1" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="68"/>
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="69" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="85"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="71"/>
     </row>
     <row r="3" spans="1:5" s="7" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="86"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
     </row>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="27" t="s">
@@ -3055,13 +3055,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="87"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
@@ -3096,13 +3096,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="88"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
     </row>
     <row r="9" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
@@ -3122,46 +3122,46 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="58" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="67"/>
+      <c r="A10" s="76"/>
       <c r="B10" s="57" t="s">
         <v>170</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="77">
         <v>0</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="73" t="s">
+      <c r="E10" s="82" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="58" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="67"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="74"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="83"/>
     </row>
     <row r="12" spans="1:5" s="58" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="67"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="68"/>
-      <c r="E12" s="74"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="83"/>
     </row>
     <row r="13" spans="1:5" s="58" customFormat="1" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="67"/>
+      <c r="A13" s="76"/>
       <c r="B13" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="75"/>
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="84"/>
     </row>
     <row r="14" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
@@ -3392,17 +3392,17 @@
         <v>96</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="70" t="s">
+      <c r="A30" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="70"/>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
+      <c r="B30" s="79"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
     </row>
     <row r="31" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30" t="s">
@@ -3452,16 +3452,16 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="81" t="s">
         <v>132</v>
       </c>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
+      <c r="B34" s="79"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="79"/>
     </row>
     <row r="35" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="71" t="s">
+      <c r="A35" s="80" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="30" t="s">
@@ -3472,7 +3472,7 @@
       <c r="E35" s="24"/>
     </row>
     <row r="36" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="71"/>
+      <c r="A36" s="80"/>
       <c r="B36" s="30" t="s">
         <v>23</v>
       </c>
@@ -3481,7 +3481,7 @@
       <c r="E36" s="24"/>
     </row>
     <row r="37" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="71"/>
+      <c r="A37" s="80"/>
       <c r="B37" s="30" t="s">
         <v>24</v>
       </c>
@@ -3669,13 +3669,13 @@
       </c>
     </row>
     <row r="53" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="70" t="s">
+      <c r="A53" s="79" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="70"/>
-      <c r="C53" s="70"/>
-      <c r="D53" s="70"/>
-      <c r="E53" s="70"/>
+      <c r="B53" s="79"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
     </row>
     <row r="54" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="30" t="s">
@@ -3782,29 +3782,29 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="79"/>
-      <c r="B62" s="79"/>
-      <c r="C62" s="79"/>
-      <c r="D62" s="79"/>
+      <c r="A62" s="88"/>
+      <c r="B62" s="88"/>
+      <c r="C62" s="88"/>
+      <c r="D62" s="88"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" s="26" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="66" t="s">
+      <c r="A63" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="B63" s="66"/>
-      <c r="C63" s="66"/>
-      <c r="D63" s="66"/>
-      <c r="E63" s="66"/>
+      <c r="B63" s="75"/>
+      <c r="C63" s="75"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
     </row>
     <row r="64" spans="1:5" s="26" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A64" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="B64" s="66"/>
-      <c r="C64" s="66"/>
-      <c r="D64" s="66"/>
-      <c r="E64" s="66"/>
+      <c r="A64" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B64" s="75"/>
+      <c r="C64" s="75"/>
+      <c r="D64" s="75"/>
+      <c r="E64" s="75"/>
     </row>
     <row r="65" spans="1:5" s="26" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="65"/>
@@ -3814,36 +3814,31 @@
       <c r="E65" s="65"/>
     </row>
     <row r="66" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="77" t="s">
+      <c r="A66" s="86" t="s">
         <v>166</v>
       </c>
-      <c r="B66" s="78"/>
-      <c r="C66" s="78"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="78"/>
+      <c r="B66" s="87"/>
+      <c r="C66" s="87"/>
+      <c r="D66" s="87"/>
+      <c r="E66" s="87"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="76" t="s">
+      <c r="A67" s="85" t="s">
         <v>168</v>
       </c>
-      <c r="B67" s="76"/>
-      <c r="C67" s="76"/>
-      <c r="D67" s="76"/>
-      <c r="E67" s="76"/>
+      <c r="B67" s="85"/>
+      <c r="C67" s="85"/>
+      <c r="D67" s="85"/>
+      <c r="E67" s="85"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="69" t="s">
+      <c r="A68" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="B68" s="69"/>
+      <c r="B68" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A8:E8"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A10:A13"/>
     <mergeCell ref="C10:C13"/>
@@ -3858,6 +3853,11 @@
     <mergeCell ref="A62:D62"/>
     <mergeCell ref="A53:E53"/>
     <mergeCell ref="A64:E64"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3868,8 +3868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A68" sqref="A67:E68"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,29 +3882,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="6" customFormat="1" ht="37.5" x14ac:dyDescent="0.7">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="97"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="91"/>
     </row>
     <row r="2" spans="1:5" s="7" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="92" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="99"/>
-      <c r="C2" s="99"/>
-      <c r="D2" s="99"/>
-      <c r="E2" s="100"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" spans="1:5" s="7" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="104"/>
-      <c r="B3" s="104"/>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
+      <c r="A3" s="98"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="98"/>
     </row>
     <row r="4" spans="1:5" s="5" customFormat="1" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
@@ -3924,13 +3924,13 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="102"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="103"/>
+      <c r="B5" s="96"/>
+      <c r="C5" s="96"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="97"/>
     </row>
     <row r="6" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -3965,13 +3965,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="102"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="103"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="97"/>
     </row>
     <row r="9" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
@@ -3991,46 +3991,46 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="105"/>
+      <c r="A10" s="99"/>
       <c r="B10" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="106">
+      <c r="C10" s="100">
         <v>0</v>
       </c>
-      <c r="D10" s="89" t="s">
+      <c r="D10" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="92" t="s">
+      <c r="E10" s="108" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="105"/>
+      <c r="A11" s="99"/>
       <c r="B11" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="107"/>
-      <c r="D11" s="90"/>
-      <c r="E11" s="93"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="106"/>
+      <c r="E11" s="109"/>
     </row>
     <row r="12" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="105"/>
+      <c r="A12" s="99"/>
       <c r="B12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="107"/>
-      <c r="D12" s="90"/>
-      <c r="E12" s="93"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="109"/>
     </row>
     <row r="13" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="105"/>
+      <c r="A13" s="99"/>
       <c r="B13" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="107"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="94"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="110"/>
     </row>
     <row r="14" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
@@ -4250,13 +4250,13 @@
       <c r="E28" s="36"/>
     </row>
     <row r="29" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="101" t="s">
+      <c r="A29" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="102"/>
-      <c r="C29" s="102"/>
-      <c r="D29" s="102"/>
-      <c r="E29" s="103"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="97"/>
     </row>
     <row r="30" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
@@ -4306,16 +4306,16 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="101" t="s">
+      <c r="A33" s="95" t="s">
         <v>133</v>
       </c>
-      <c r="B33" s="102"/>
-      <c r="C33" s="102"/>
-      <c r="D33" s="102"/>
-      <c r="E33" s="103"/>
+      <c r="B33" s="96"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="97"/>
     </row>
     <row r="34" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="109" t="s">
+      <c r="A34" s="103" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="17" t="s">
@@ -4326,7 +4326,7 @@
       <c r="E34" s="36"/>
     </row>
     <row r="35" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="109"/>
+      <c r="A35" s="103"/>
       <c r="B35" s="17" t="s">
         <v>69</v>
       </c>
@@ -4335,7 +4335,7 @@
       <c r="E35" s="36"/>
     </row>
     <row r="36" spans="1:5" ht="33.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="109"/>
+      <c r="A36" s="103"/>
       <c r="B36" s="16" t="s">
         <v>70</v>
       </c>
@@ -4523,13 +4523,13 @@
       </c>
     </row>
     <row r="52" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="101" t="s">
+      <c r="A52" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="B52" s="102"/>
-      <c r="C52" s="102"/>
-      <c r="D52" s="102"/>
-      <c r="E52" s="103"/>
+      <c r="B52" s="96"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="97"/>
     </row>
     <row r="53" spans="1:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
@@ -4636,29 +4636,29 @@
       </c>
     </row>
     <row r="61" spans="1:5" ht="17.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="110"/>
-      <c r="B61" s="110"/>
-      <c r="C61" s="110"/>
+      <c r="A61" s="104"/>
+      <c r="B61" s="104"/>
+      <c r="C61" s="104"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
     </row>
     <row r="62" spans="1:5" s="26" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="66" t="s">
+      <c r="A62" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="B62" s="66"/>
-      <c r="C62" s="66"/>
-      <c r="D62" s="66"/>
-      <c r="E62" s="66"/>
+      <c r="B62" s="75"/>
+      <c r="C62" s="75"/>
+      <c r="D62" s="75"/>
+      <c r="E62" s="75"/>
     </row>
     <row r="63" spans="1:5" s="26" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A63" s="66" t="s">
-        <v>181</v>
-      </c>
-      <c r="B63" s="66"/>
-      <c r="C63" s="66"/>
-      <c r="D63" s="66"/>
-      <c r="E63" s="66"/>
+      <c r="A63" s="75" t="s">
+        <v>180</v>
+      </c>
+      <c r="B63" s="75"/>
+      <c r="C63" s="75"/>
+      <c r="D63" s="75"/>
+      <c r="E63" s="75"/>
     </row>
     <row r="64" spans="1:5" s="26" customFormat="1" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A64" s="65"/>
@@ -4668,43 +4668,49 @@
       <c r="E64" s="65"/>
     </row>
     <row r="65" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="77" t="s">
+      <c r="A65" s="86" t="s">
         <v>166</v>
       </c>
-      <c r="B65" s="78"/>
-      <c r="C65" s="78"/>
-      <c r="D65" s="78"/>
-      <c r="E65" s="78"/>
+      <c r="B65" s="87"/>
+      <c r="C65" s="87"/>
+      <c r="D65" s="87"/>
+      <c r="E65" s="87"/>
     </row>
     <row r="66" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="77" t="s">
+      <c r="A66" s="86" t="s">
         <v>167</v>
       </c>
-      <c r="B66" s="78"/>
-      <c r="C66" s="78"/>
-      <c r="D66" s="78"/>
-      <c r="E66" s="78"/>
+      <c r="B66" s="87"/>
+      <c r="C66" s="87"/>
+      <c r="D66" s="87"/>
+      <c r="E66" s="87"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="76" t="s">
+      <c r="A67" s="85" t="s">
         <v>168</v>
       </c>
-      <c r="B67" s="76"/>
-      <c r="C67" s="76"/>
-      <c r="D67" s="76"/>
-      <c r="E67" s="76"/>
+      <c r="B67" s="85"/>
+      <c r="C67" s="85"/>
+      <c r="D67" s="85"/>
+      <c r="E67" s="85"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="69" t="s">
+      <c r="A68" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="B68" s="69"/>
+      <c r="B68" s="78"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="A67:E67"/>
+    <mergeCell ref="A63:E63"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A5:E5"/>
@@ -4719,12 +4725,6 @@
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A61:C61"/>
     <mergeCell ref="A52:E52"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="E10:E13"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A63:E63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>